<commit_message>
Learned 2 more Functions
</commit_message>
<xml_diff>
--- a/2_Intermediate Excel.xlsx
+++ b/2_Intermediate Excel.xlsx
@@ -1,70 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/632ee06d642e1deb/Desktop/EXCEL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA ENGINEERING\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{777136D3-E182-4A77-8688-AA03CAE4B5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B36C851-33C3-4462-85A0-EFF60976D724}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED1A742-1C72-4EE5-BA31-FCAB25E2B631}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="14" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" firstSheet="15" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Maths &amp; Trigo (SUM PRODUCT)" sheetId="1" r:id="rId1"/>
-    <sheet name="MROUND" sheetId="2" r:id="rId2"/>
-    <sheet name="Floor" sheetId="3" r:id="rId3"/>
-    <sheet name="Ceiling" sheetId="4" r:id="rId4"/>
-    <sheet name="Mod" sheetId="5" r:id="rId5"/>
-    <sheet name="Quotient" sheetId="6" r:id="rId6"/>
-    <sheet name="VLOOKUP" sheetId="7" r:id="rId7"/>
-    <sheet name="Vlookup Approximate Match" sheetId="8" r:id="rId8"/>
-    <sheet name="Vlookup with Trim" sheetId="9" r:id="rId9"/>
-    <sheet name="H Lookup" sheetId="10" r:id="rId10"/>
-    <sheet name="Match Function" sheetId="11" r:id="rId11"/>
-    <sheet name="Index Function" sheetId="12" r:id="rId12"/>
-    <sheet name="Lock Unlock Cells" sheetId="13" r:id="rId13"/>
-    <sheet name="Unlock Entire Sheets" sheetId="14" r:id="rId14"/>
-    <sheet name="Protect and Unprotect Sheets" sheetId="15" r:id="rId15"/>
-    <sheet name="Protect File" sheetId="16" r:id="rId16"/>
-    <sheet name="Protect Workbook" sheetId="17" r:id="rId17"/>
-    <sheet name="Hyperlink to sheet" sheetId="18" r:id="rId18"/>
+    <sheet name="1_Maths &amp; Trigo (SUM PRODUCT)" sheetId="1" r:id="rId1"/>
+    <sheet name="2_MROUND" sheetId="2" r:id="rId2"/>
+    <sheet name="3_Floor" sheetId="3" r:id="rId3"/>
+    <sheet name="4_ Ceiling" sheetId="4" r:id="rId4"/>
+    <sheet name="5_Mod" sheetId="5" r:id="rId5"/>
+    <sheet name="6_Quotient" sheetId="6" r:id="rId6"/>
+    <sheet name="7_VLOOKUP" sheetId="7" r:id="rId7"/>
+    <sheet name="8_Vlookup Approximate Match" sheetId="8" r:id="rId8"/>
+    <sheet name="9_Vlookup with Trim" sheetId="9" r:id="rId9"/>
+    <sheet name="10_H Lookup" sheetId="10" r:id="rId10"/>
+    <sheet name="11_Match Function" sheetId="11" r:id="rId11"/>
+    <sheet name="12_Index Function" sheetId="12" r:id="rId12"/>
+    <sheet name="13_Lock Unlock Cells" sheetId="13" r:id="rId13"/>
+    <sheet name="14_Unlock Entire Sheets" sheetId="14" r:id="rId14"/>
+    <sheet name="15_Protect and Unprotect Sheets" sheetId="15" r:id="rId15"/>
+    <sheet name="16_Protect File" sheetId="16" r:id="rId16"/>
+    <sheet name="17_Protect Workbook" sheetId="17" r:id="rId17"/>
+    <sheet name="18_Hyperlink to sheet" sheetId="18" r:id="rId18"/>
     <sheet name="Hyperlinked" sheetId="19" r:id="rId19"/>
-    <sheet name="Sheet4" sheetId="20" r:id="rId20"/>
+    <sheet name="3" sheetId="20" r:id="rId20"/>
   </sheets>
   <definedNames>
-    <definedName name="Table">VLOOKUP!$A$5:$D$12</definedName>
+    <definedName name="Table">'7_VLOOKUP'!$A$5:$D$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -79,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="109">
   <si>
     <t>Array 1</t>
   </si>
@@ -394,6 +384,18 @@
   </si>
   <si>
     <t>Go to Webpage</t>
+  </si>
+  <si>
+    <t>Press Contol 1 to get Format cell</t>
+  </si>
+  <si>
+    <t>By Default all Cells are Locked</t>
+  </si>
+  <si>
+    <t>Right Click on the Sheet and Unprotect it</t>
+  </si>
+  <si>
+    <t>go to</t>
   </si>
 </sst>
 </file>
@@ -546,6 +548,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -559,7 +562,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -580,6 +582,54 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>46768</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24260AFC-4F0F-4ECC-9CE4-901C4F60F433}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="37895" t="54590" r="48510" b="1389"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5838825" y="2933700"/>
+          <a:ext cx="1657350" cy="3018568"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -902,22 +952,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D7"/>
+  <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+    <row r="2" spans="2:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-    </row>
-    <row r="3" spans="2:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+    </row>
+    <row r="3" spans="2:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -928,7 +978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>3</v>
       </c>
@@ -940,7 +990,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>8</v>
       </c>
@@ -948,11 +998,11 @@
         <v>6</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D6" si="0">B5*C5</f>
+        <f>B5*C5</f>
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>1</v>
       </c>
@@ -960,15 +1010,21 @@
         <v>5</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="0"/>
+        <f>B6*C6</f>
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3">
         <f>SUMPRODUCT(B4:B6,C4:C6)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f>SUMPRODUCT(B4:B7,C4:C7)</f>
         <v>59</v>
       </c>
     </row>
@@ -985,31 +1041,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABEBAD6-5B7A-456F-8464-60E7BB096317}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>42</v>
       </c>
@@ -1032,7 +1088,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>23</v>
       </c>
@@ -1055,7 +1111,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>24</v>
       </c>
@@ -1078,7 +1134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>25</v>
       </c>
@@ -1101,7 +1157,7 @@
         <v>20.95</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>42</v>
       </c>
@@ -1109,7 +1165,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
@@ -1134,27 +1190,27 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B14"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1165,49 +1221,49 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F6">
         <f>MATCH(E6,B6:B13,)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>34</v>
       </c>
@@ -1223,22 +1279,22 @@
   <dimension ref="B2:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
@@ -1252,7 +1308,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str" cm="1">
         <f t="array" ref="B3:E10">Table</f>
         <v>Mobile</v>
@@ -1267,7 +1323,7 @@
         <v>26.95</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <v>Camera</v>
       </c>
@@ -1287,7 +1343,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <v>Watches</v>
       </c>
@@ -1300,15 +1356,15 @@
       <c r="E5" s="3">
         <v>31.95</v>
       </c>
-      <c r="H5" s="3" t="str" cm="1">
-        <f t="array" ref="H5">INDEX(B3:B10,I5)</f>
+      <c r="H5" s="3" t="str">
+        <f>INDEX(B3:B10,I5)</f>
         <v>Shoes</v>
       </c>
       <c r="I5" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="str">
         <v>Cosmetics</v>
       </c>
@@ -1322,7 +1378,7 @@
         <v>35.950000000000003</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <v>Shoes</v>
       </c>
@@ -1345,7 +1401,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <v>Laptop</v>
       </c>
@@ -1369,7 +1425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <v>Perfumes</v>
       </c>
@@ -1383,7 +1439,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="str">
         <v>Clothes</v>
       </c>
@@ -1397,7 +1453,7 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>87</v>
       </c>
@@ -1410,26 +1466,26 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3B2585-E2C1-4E47-9942-B194998A0F26}">
-  <dimension ref="B2:E15"/>
+  <dimension ref="B2:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="24" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
         <v>42</v>
       </c>
@@ -1437,41 +1493,50 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="20" t="s">
         <v>32</v>
       </c>
@@ -1479,7 +1544,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
         <v>33</v>
       </c>
@@ -1487,7 +1552,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
         <v>34</v>
       </c>
@@ -1495,12 +1560,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E14" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E15" s="3" t="s">
         <v>94</v>
       </c>
@@ -1519,25 +1584,25 @@
   <dimension ref="A2:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="21"/>
-    <col min="4" max="4" width="30.109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="21"/>
+    <col min="1" max="1" width="11.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="21"/>
+    <col min="4" max="4" width="30.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1545,7 +1610,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1553,7 +1618,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
@@ -1561,7 +1626,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
@@ -1569,17 +1634,17 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
@@ -1587,7 +1652,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -1595,7 +1660,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
@@ -1603,12 +1668,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" s="20" t="s">
         <v>94</v>
       </c>
@@ -1628,22 +1693,22 @@
   <dimension ref="C4:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="24" t="s">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" s="19" t="s">
         <v>42</v>
       </c>
@@ -1651,7 +1716,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" s="20" t="s">
         <v>26</v>
       </c>
@@ -1659,11 +1724,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" s="20"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" s="20" t="s">
         <v>28</v>
       </c>
@@ -1671,7 +1736,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" s="20" t="s">
         <v>29</v>
       </c>
@@ -1679,17 +1744,17 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C12" s="20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C13" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C14" s="20" t="s">
         <v>32</v>
       </c>
@@ -1697,7 +1762,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C15" s="20" t="s">
         <v>33</v>
       </c>
@@ -1705,7 +1770,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C16" s="20" t="s">
         <v>34</v>
       </c>
@@ -1713,12 +1778,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18" s="3" t="s">
         <v>94</v>
       </c>
@@ -1730,6 +1795,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1738,30 +1804,30 @@
   <dimension ref="C4:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="24" t="s">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D5" s="24" t="s">
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" s="19" t="s">
         <v>42</v>
       </c>
@@ -1769,7 +1835,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" s="20" t="s">
         <v>26</v>
       </c>
@@ -1777,11 +1843,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" s="20"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" s="20" t="s">
         <v>28</v>
       </c>
@@ -1789,7 +1855,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" s="20" t="s">
         <v>29</v>
       </c>
@@ -1797,17 +1863,17 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C12" s="20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C13" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C14" s="20" t="s">
         <v>32</v>
       </c>
@@ -1815,7 +1881,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C15" s="20" t="s">
         <v>33</v>
       </c>
@@ -1823,7 +1889,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C16" s="20" t="s">
         <v>34</v>
       </c>
@@ -1831,17 +1897,18 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18" s="3" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection password="CF7A" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D5:F5"/>
@@ -1855,9 +1922,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCC3999-025F-4725-823F-102A83CA09F0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1869,39 +1938,44 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:C7"/>
+  <dimension ref="B3:C9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C3" s="26" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="22" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C4" s="26" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="22" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C5" s="26" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="22" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>100</v>
       </c>
       <c r="C7" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1923,11 +1997,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE827AB-5490-426D-B036-9B97BE460FB2}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.25" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1945,17 +2019,17 @@
   <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1969,7 +2043,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>4.4000000000000004</v>
       </c>
@@ -1984,7 +2058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>7.5</v>
       </c>
@@ -1999,7 +2073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>24</v>
       </c>
@@ -2014,7 +2088,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>11</v>
       </c>
@@ -2033,7 +2107,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2045,15 +2119,15 @@
   <dimension ref="B2:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B2" sqref="B2:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2067,7 +2141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>3.9</v>
       </c>
@@ -2082,7 +2156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>9</v>
       </c>
@@ -2097,7 +2171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>21</v>
       </c>
@@ -2112,12 +2186,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>18</v>
       </c>
@@ -2130,12 +2204,74 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45635E44-EAC8-47DC-81AD-BCCCC31AE259}">
-  <dimension ref="A1"/>
+  <dimension ref="B3:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3">
+        <f>_xlfn.FLOOR.MATH(B4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3">
+        <f>_xlfn.FLOOR.MATH(B5,5)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3">
+        <f>_xlfn.FLOOR.MATH(B6,3)</f>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2146,17 +2282,17 @@
   <dimension ref="C2:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D4">
         <f>MOD(50,3)</f>
         <v>2</v>
@@ -2173,12 +2309,12 @@
   <dimension ref="C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C3">
         <f>QUOTIENT(5,2)</f>
         <v>2</v>
@@ -2194,23 +2330,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFD0811-4504-4E53-8F72-FFF6E0E96DD2}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="80.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="80.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -2222,7 +2360,7 @@
         <v>18.95</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F3" s="18" t="s">
         <v>74</v>
       </c>
@@ -2230,7 +2368,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -2250,7 +2388,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
@@ -2270,7 +2408,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
@@ -2290,7 +2428,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>29</v>
       </c>
@@ -2304,7 +2442,7 @@
         <v>31.95</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
@@ -2318,7 +2456,7 @@
         <v>35.950000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>31</v>
       </c>
@@ -2332,7 +2470,7 @@
         <v>18.95</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>32</v>
       </c>
@@ -2346,7 +2484,7 @@
         <v>20.95</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>33</v>
       </c>
@@ -2360,7 +2498,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>34</v>
       </c>
@@ -2373,8 +2511,11 @@
       <c r="D12" s="7">
         <v>8.9499999999999993</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>42</v>
       </c>
@@ -2388,7 +2529,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>33</v>
       </c>
@@ -2404,15 +2545,15 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="23" t="s">
+    <row r="17" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-    </row>
-    <row r="18" spans="1:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+    </row>
+    <row r="18" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>45</v>
       </c>
@@ -2420,7 +2561,7 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>46</v>
       </c>
@@ -2434,28 +2575,28 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B20" s="9">
         <f>VLOOKUP(A20,Table,4,)</f>
-        <v>4.95</v>
+        <v>31.95</v>
       </c>
       <c r="C20" s="3">
         <v>5</v>
       </c>
       <c r="D20" s="9">
         <f>C20*B20</f>
-        <v>24.75</v>
+        <v>159.75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A17:D17"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A20" xr:uid="{AB4B757F-A61E-4F54-A293-FCE31DFBF127}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A20 G12" xr:uid="{AB4B757F-A61E-4F54-A293-FCE31DFBF127}">
       <formula1>$A$5:$A$12</formula1>
     </dataValidation>
   </dataValidations>
@@ -2468,23 +2609,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B53DCC-24DF-4E5D-AD3E-83EC1D9D8872}">
   <dimension ref="B2:E17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>49</v>
       </c>
@@ -2498,7 +2639,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>50</v>
       </c>
@@ -2512,7 +2653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>51</v>
       </c>
@@ -2526,7 +2667,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>52</v>
       </c>
@@ -2540,7 +2681,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>53</v>
       </c>
@@ -2554,7 +2695,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>54</v>
       </c>
@@ -2568,23 +2709,23 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
         <v>65</v>
       </c>
       <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
         <v>63</v>
       </c>
@@ -2592,13 +2733,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="16">
-        <v>40</v>
+        <v>1000000</v>
       </c>
       <c r="C17" s="3">
         <f>VLOOKUP(B17,C5:E9,3,1)</f>
-        <v>0</v>
+        <v>1400</v>
       </c>
     </row>
   </sheetData>
@@ -2611,25 +2752,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F480D3E-6B9D-46E9-9900-790980238AFB}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
         <v>42</v>
       </c>
@@ -2643,7 +2784,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str" cm="1">
         <f t="array" ref="B4:E11">Table</f>
         <v>Mobile</v>
@@ -2658,7 +2799,7 @@
         <v>26.95</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <v>Camera</v>
       </c>
@@ -2672,7 +2813,7 @@
         <v>28.95</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="str">
         <v>Watches</v>
       </c>
@@ -2686,7 +2827,7 @@
         <v>31.95</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <v>Cosmetics</v>
       </c>
@@ -2700,7 +2841,7 @@
         <v>35.950000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <v>Shoes</v>
       </c>
@@ -2714,7 +2855,7 @@
         <v>18.95</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <v>Laptop</v>
       </c>
@@ -2728,7 +2869,7 @@
         <v>20.95</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="str">
         <v>Perfumes</v>
       </c>
@@ -2742,7 +2883,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="str">
         <v>Clothes</v>
       </c>
@@ -2756,12 +2897,12 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
         <v>42</v>
       </c>
@@ -2769,7 +2910,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>70</v>
       </c>
@@ -2778,7 +2919,7 @@
         <v>26.95</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>71</v>
       </c>
@@ -2787,7 +2928,7 @@
         <v>28.95</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>29</v>
       </c>
@@ -2796,7 +2937,7 @@
         <v>31.95</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
@@ -2805,7 +2946,7 @@
         <v>35.950000000000003</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>31</v>
       </c>
@@ -2814,7 +2955,7 @@
         <v>18.95</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>32</v>
       </c>
@@ -2823,7 +2964,7 @@
         <v>20.95</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>33</v>
       </c>
@@ -2832,7 +2973,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>34</v>
       </c>

</xml_diff>